<commit_message>
Theme Glow, adding remaining files
</commit_message>
<xml_diff>
--- a/Themes/Links of Images Used.xlsx
+++ b/Themes/Links of Images Used.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ACFDDF-115A-40FA-B9D1-B58C21BDB730}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7699082-4CF1-4BA1-95E5-C80769422529}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>https://www.shutterstock.com/image-vector/slot-machine-spin-button-vector-illustration-314013959?src=483Q5emYoinLl46jLdqLmg-1-13</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>https://www.shutterstock.com/image-vector/slot-machine-spin-button-vector-illustration-314013929?src=483Q5emYoinLl46jLdqLmg-1-4</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>https://www.dreamstime.com/casino-theme-decorative-design-elements-chalkboard-gambling-symbols-casino-theme-decorative-design-elements-chalkboard-image105692673</t>
+  </si>
+  <si>
+    <t>Glow</t>
+  </si>
+  <si>
+    <t>https://www.shutterstock.com/image-illustration/dark-bright-pattern-playing-card-symbols-756655723?src=979Kn-kXZpVNhVXiNDOEqw-7-86</t>
   </si>
 </sst>
 </file>
@@ -385,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,6 +452,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>